<commit_message>
add namespaces to elements
</commit_message>
<xml_diff>
--- a/xls/sim_struct.xlsx
+++ b/xls/sim_struct.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="795" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="795" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="format_template" sheetId="17" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="222">
   <si>
     <t>ОРУ 500 кВ</t>
   </si>
@@ -163,28 +163,13 @@
     <t>_96521323C5CB419BA6433904BBAFC08B</t>
   </si>
   <si>
-    <t>GeographicalRegion</t>
-  </si>
-  <si>
     <t>ОЭС Центра</t>
-  </si>
-  <si>
-    <t>SubGeographicalRegion</t>
   </si>
   <si>
     <t>Брянская ЭЭС</t>
   </si>
   <si>
-    <t>Substation</t>
-  </si>
-  <si>
     <t>ПС 500 Белобережская</t>
-  </si>
-  <si>
-    <t>SubControlArea</t>
-  </si>
-  <si>
-    <t>HostControlArea</t>
   </si>
   <si>
     <t>МЭС Северо-Запада</t>
@@ -194,12 +179,6 @@
   </si>
   <si>
     <t>РДУ Северо-Запада</t>
-  </si>
-  <si>
-    <t>Company</t>
-  </si>
-  <si>
-    <t>CompanyType</t>
   </si>
   <si>
     <t>Магистральные электрические сети</t>
@@ -218,12 +197,6 @@
   </si>
   <si>
     <t>class</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>aliasName</t>
   </si>
   <si>
     <t>rdf:ID</t>
@@ -275,9 +248,6 @@
   </si>
   <si>
     <t>cim:IdentifiedObject.name</t>
-  </si>
-  <si>
-    <t>ptiColor</t>
   </si>
   <si>
     <t>id_1</t>
@@ -696,6 +666,36 @@
   <si>
     <t>name_3</t>
   </si>
+  <si>
+    <t>ТСН-2 10</t>
+  </si>
+  <si>
+    <t>cim:SubGeographicalRegion.Region</t>
+  </si>
+  <si>
+    <t>pti:BaseVoltage.ptiColor</t>
+  </si>
+  <si>
+    <t>GeographicalRegion</t>
+  </si>
+  <si>
+    <t>SubGeographicalRegion</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>CompanyType</t>
+  </si>
+  <si>
+    <t>SubControlArea</t>
+  </si>
+  <si>
+    <t>HostControlArea</t>
+  </si>
+  <si>
+    <t>Substation</t>
+  </si>
 </sst>
 </file>
 
@@ -1067,31 +1067,31 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="B4" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1255,31 +1255,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1307,10 +1307,10 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="H2" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="I2" t="s">
         <v>28</v>
@@ -1341,10 +1341,10 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="H3" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="I3" t="s">
         <v>29</v>
@@ -1375,13 +1375,13 @@
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="H4" t="s">
         <v>12</v>
       </c>
       <c r="I4" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1409,13 +1409,13 @@
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="H5" t="s">
         <v>13</v>
       </c>
       <c r="I5" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -1442,28 +1442,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1491,10 +1491,10 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="H2" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1522,10 +1522,10 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="H3" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -1560,34 +1560,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1604,7 +1604,7 @@
         <v>В-1-500 ВЛ 500 Новобрянская</v>
       </c>
       <c r="E2" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F2" t="str">
         <f>'Bay(4)'!$A$8</f>
@@ -1618,7 +1618,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="J2" t="s">
         <v>7</v>
@@ -1638,7 +1638,7 @@
         <v>В-2-500 ВЛ 500 Новобрянская</v>
       </c>
       <c r="E3" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F3" t="str">
         <f>'Bay(4)'!$A$8</f>
@@ -1652,7 +1652,7 @@
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="J3" t="s">
         <v>7</v>
@@ -1672,7 +1672,7 @@
         <v>В-1-500 ВЛ 500 Елецкая</v>
       </c>
       <c r="E4" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F4" t="str">
         <f>'Bay(4)'!$A$7</f>
@@ -1686,7 +1686,7 @@
         <v>3</v>
       </c>
       <c r="I4" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="J4" t="s">
         <v>6</v>
@@ -1706,7 +1706,7 @@
         <v>В-2-500 ВЛ 500 Елецкая</v>
       </c>
       <c r="E5" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F5" t="str">
         <f>'Bay(4)'!$A$7</f>
@@ -1720,7 +1720,7 @@
         <v>4</v>
       </c>
       <c r="I5" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="J5" t="s">
         <v>6</v>
@@ -1740,7 +1740,7 @@
         <v>В 211 ВЛ 220 Брянская</v>
       </c>
       <c r="E6" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F6" t="str">
         <f>'Bay(4)'!$A$3</f>
@@ -1754,7 +1754,7 @@
         <v>5</v>
       </c>
       <c r="I6" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="J6" t="s">
         <v>3</v>
@@ -1774,7 +1774,7 @@
         <v>В 210 ВЛ 220 Машзавод</v>
       </c>
       <c r="E7" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F7" t="str">
         <f>'Bay(4)'!$A$5</f>
@@ -1788,7 +1788,7 @@
         <v>6</v>
       </c>
       <c r="I7" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="J7" t="s">
         <v>4</v>
@@ -1808,7 +1808,7 @@
         <v>В 212 ВЛ 220 Машзавод</v>
       </c>
       <c r="E8" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F8" t="str">
         <f>'Bay(4)'!$A$5</f>
@@ -1822,7 +1822,7 @@
         <v>7</v>
       </c>
       <c r="I8" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="J8" t="s">
         <v>4</v>
@@ -1842,7 +1842,7 @@
         <v>В 220 ВЛ 220 Цементная</v>
       </c>
       <c r="E9" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F9" t="str">
         <f>'Bay(4)'!$A$6</f>
@@ -1856,7 +1856,7 @@
         <v>8</v>
       </c>
       <c r="I9" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="J9" t="s">
         <v>5</v>
@@ -1876,7 +1876,7 @@
         <v>В 221 ВЛ 220 Цементная</v>
       </c>
       <c r="E10" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F10" t="str">
         <f>'Bay(4)'!$A$6</f>
@@ -1890,7 +1890,7 @@
         <v>9</v>
       </c>
       <c r="I10" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="J10" t="s">
         <v>5</v>
@@ -1910,7 +1910,7 @@
         <v>В 10 AT-1</v>
       </c>
       <c r="E11" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F11" t="str">
         <f>'Bay(4)'!$A$2</f>
@@ -1924,7 +1924,7 @@
         <v>10</v>
       </c>
       <c r="I11" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="J11" t="s">
         <v>8</v>
@@ -1944,7 +1944,7 @@
         <v>В 10 AT-2</v>
       </c>
       <c r="E12" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F12" t="str">
         <f>'Bay(4)'!$A$3</f>
@@ -1958,7 +1958,7 @@
         <v>11</v>
       </c>
       <c r="I12" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="J12" t="s">
         <v>9</v>
@@ -1978,7 +1978,7 @@
         <v xml:space="preserve">СВ 10 </v>
       </c>
       <c r="E13" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F13" t="str">
         <f>'Bay(4)'!$A$13</f>
@@ -2009,7 +2009,7 @@
         <v>В 10 ТСН-1</v>
       </c>
       <c r="E14" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F14" t="str">
         <f>'Bay(4)'!$A$11</f>
@@ -2023,7 +2023,7 @@
         <v>13</v>
       </c>
       <c r="I14" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="J14" t="s">
         <v>12</v>
@@ -2043,7 +2043,7 @@
         <v>В 10 ТСН-2</v>
       </c>
       <c r="E15" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F15" t="str">
         <f>'Bay(4)'!$A$12</f>
@@ -2057,7 +2057,7 @@
         <v>14</v>
       </c>
       <c r="I15" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="J15" t="s">
         <v>13</v>
@@ -2090,34 +2090,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -2138,7 +2138,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E2" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F2" t="str">
         <f>'Bay(4)'!$A$8</f>
@@ -2152,7 +2152,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="J2" t="s">
         <v>7</v>
@@ -2176,7 +2176,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E3" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F3" t="str">
         <f>'Bay(4)'!$A$8</f>
@@ -2190,7 +2190,7 @@
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="J3" t="s">
         <v>7</v>
@@ -2214,7 +2214,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E4" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F4" t="str">
         <f>'Bay(4)'!$A$8</f>
@@ -2228,7 +2228,7 @@
         <v>3</v>
       </c>
       <c r="I4" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="J4" t="s">
         <v>7</v>
@@ -2252,7 +2252,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E5" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F5" t="str">
         <f>'Bay(4)'!$A$8</f>
@@ -2266,7 +2266,7 @@
         <v>4</v>
       </c>
       <c r="I5" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="J5" t="s">
         <v>7</v>
@@ -2290,7 +2290,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E6" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F6" t="str">
         <f>'Bay(4)'!$A$8</f>
@@ -2304,7 +2304,7 @@
         <v>5</v>
       </c>
       <c r="I6" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="J6" t="s">
         <v>7</v>
@@ -2328,7 +2328,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E7" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F7" t="str">
         <f>'Bay(4)'!$A$7</f>
@@ -2342,7 +2342,7 @@
         <v>6</v>
       </c>
       <c r="I7" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="J7" t="s">
         <v>6</v>
@@ -2366,7 +2366,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E8" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F8" t="str">
         <f>'Bay(4)'!$A$7</f>
@@ -2380,7 +2380,7 @@
         <v>7</v>
       </c>
       <c r="I8" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="J8" t="s">
         <v>6</v>
@@ -2404,7 +2404,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E9" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F9" t="str">
         <f>'Bay(4)'!$A$7</f>
@@ -2418,7 +2418,7 @@
         <v>8</v>
       </c>
       <c r="I9" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="J9" t="s">
         <v>6</v>
@@ -2442,7 +2442,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E10" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F10" t="str">
         <f>'Bay(4)'!$A$7</f>
@@ -2456,7 +2456,7 @@
         <v>9</v>
       </c>
       <c r="I10" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="J10" t="s">
         <v>6</v>
@@ -2480,7 +2480,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E11" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F11" t="str">
         <f>'Bay(4)'!$A$7</f>
@@ -2494,7 +2494,7 @@
         <v>10</v>
       </c>
       <c r="I11" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="J11" t="s">
         <v>6</v>
@@ -2518,7 +2518,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E12" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F12" t="str">
         <f>'Bay(4)'!$A$2</f>
@@ -2532,7 +2532,7 @@
         <v>11</v>
       </c>
       <c r="I12" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="J12" t="s">
         <v>8</v>
@@ -2556,7 +2556,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E13" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F13" t="str">
         <f>'Bay(4)'!$A$3</f>
@@ -2570,7 +2570,7 @@
         <v>12</v>
       </c>
       <c r="I13" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="J13" t="s">
         <v>9</v>
@@ -2594,7 +2594,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E14" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F14" t="str">
         <f>'Bay(4)'!$A$2</f>
@@ -2608,7 +2608,7 @@
         <v>13</v>
       </c>
       <c r="I14" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="J14" t="s">
         <v>8</v>
@@ -2632,7 +2632,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E15" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F15" t="str">
         <f>'Bay(4)'!$A$3</f>
@@ -2646,7 +2646,7 @@
         <v>14</v>
       </c>
       <c r="I15" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="J15" t="s">
         <v>9</v>
@@ -2670,7 +2670,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E16" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F16" t="str">
         <f>'Bay(4)'!$A$3</f>
@@ -2684,7 +2684,7 @@
         <v>15</v>
       </c>
       <c r="I16" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="J16" t="s">
         <v>3</v>
@@ -2708,7 +2708,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E17" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F17" t="str">
         <f>'Bay(4)'!$A$3</f>
@@ -2722,7 +2722,7 @@
         <v>16</v>
       </c>
       <c r="I17" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="J17" t="s">
         <v>3</v>
@@ -2746,7 +2746,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E18" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F18" t="str">
         <f>'Bay(4)'!$A$3</f>
@@ -2760,7 +2760,7 @@
         <v>17</v>
       </c>
       <c r="I18" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="J18" t="s">
         <v>3</v>
@@ -2784,7 +2784,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E19" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F19" t="str">
         <f>'Bay(4)'!$A$5</f>
@@ -2798,7 +2798,7 @@
         <v>18</v>
       </c>
       <c r="I19" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="J19" t="s">
         <v>4</v>
@@ -2822,7 +2822,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E20" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F20" t="str">
         <f>'Bay(4)'!$A$5</f>
@@ -2836,7 +2836,7 @@
         <v>19</v>
       </c>
       <c r="I20" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="J20" t="s">
         <v>4</v>
@@ -2860,7 +2860,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E21" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F21" t="str">
         <f>'Bay(4)'!$A$5</f>
@@ -2874,7 +2874,7 @@
         <v>20</v>
       </c>
       <c r="I21" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="J21" t="s">
         <v>4</v>
@@ -2898,7 +2898,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E22" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F22" t="str">
         <f>'Bay(4)'!$A$5</f>
@@ -2912,7 +2912,7 @@
         <v>21</v>
       </c>
       <c r="I22" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="J22" t="s">
         <v>4</v>
@@ -2936,7 +2936,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E23" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F23" t="str">
         <f>'Bay(4)'!$A$5</f>
@@ -2950,7 +2950,7 @@
         <v>22</v>
       </c>
       <c r="I23" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="J23" t="s">
         <v>4</v>
@@ -2974,7 +2974,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E24" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F24" t="str">
         <f>'Bay(4)'!$A$6</f>
@@ -2988,7 +2988,7 @@
         <v>23</v>
       </c>
       <c r="I24" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="J24" t="s">
         <v>5</v>
@@ -3012,7 +3012,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E25" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F25" t="str">
         <f>'Bay(4)'!$A$6</f>
@@ -3026,7 +3026,7 @@
         <v>24</v>
       </c>
       <c r="I25" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="J25" t="s">
         <v>5</v>
@@ -3050,7 +3050,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E26" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F26" t="str">
         <f>'Bay(4)'!$A$6</f>
@@ -3064,7 +3064,7 @@
         <v>25</v>
       </c>
       <c r="I26" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="J26" t="s">
         <v>5</v>
@@ -3088,7 +3088,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E27" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F27" t="str">
         <f>'Bay(4)'!$A$6</f>
@@ -3102,7 +3102,7 @@
         <v>26</v>
       </c>
       <c r="I27" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="J27" t="s">
         <v>5</v>
@@ -3126,7 +3126,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E28" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F28" t="str">
         <f>'Bay(4)'!$A$6</f>
@@ -3140,7 +3140,7 @@
         <v>27</v>
       </c>
       <c r="I28" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="J28" t="s">
         <v>5</v>
@@ -3164,7 +3164,7 @@
         <v>_327A14C3DF4C44D691FD4E1B480EBE15</v>
       </c>
       <c r="E29" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F29" t="str">
         <f>'Bay(4)'!$A$14</f>
@@ -3178,7 +3178,7 @@
         <v>28</v>
       </c>
       <c r="I29" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="J29" t="s">
         <v>15</v>
@@ -3211,34 +3211,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -3259,7 +3259,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E2" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F2" t="str">
         <f>'BusbarSection(5)'!$A$10</f>
@@ -3273,7 +3273,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="J2" t="s">
         <v>17</v>
@@ -3297,7 +3297,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E3" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F3" t="str">
         <f>'BusbarSection(5)'!$A$10</f>
@@ -3311,7 +3311,7 @@
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="J3" t="s">
         <v>17</v>
@@ -3335,7 +3335,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E4" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F4" t="str">
         <f>'Bay(4)'!$A$8</f>
@@ -3349,7 +3349,7 @@
         <v>3</v>
       </c>
       <c r="I4" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="J4" t="s">
         <v>7</v>
@@ -3373,7 +3373,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E5" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F5" t="str">
         <f>'Bay(4)'!$A$8</f>
@@ -3387,7 +3387,7 @@
         <v>4</v>
       </c>
       <c r="I5" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="J5" t="s">
         <v>7</v>
@@ -3411,7 +3411,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E6" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F6" t="str">
         <f>'Bay(4)'!$A$8</f>
@@ -3425,7 +3425,7 @@
         <v>5</v>
       </c>
       <c r="I6" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="J6" t="s">
         <v>7</v>
@@ -3449,7 +3449,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E7" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F7" t="str">
         <f>'Bay(4)'!$A$8</f>
@@ -3463,7 +3463,7 @@
         <v>6</v>
       </c>
       <c r="I7" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="J7" t="s">
         <v>7</v>
@@ -3487,7 +3487,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E8" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F8" t="str">
         <f>'Bay(4)'!$A$8</f>
@@ -3501,7 +3501,7 @@
         <v>7</v>
       </c>
       <c r="I8" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="J8" t="s">
         <v>7</v>
@@ -3525,7 +3525,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E9" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F9" t="str">
         <f>'Bay(4)'!$A$8</f>
@@ -3539,7 +3539,7 @@
         <v>8</v>
       </c>
       <c r="I9" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="J9" t="s">
         <v>7</v>
@@ -3563,7 +3563,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E10" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F10" t="str">
         <f>'Bay(4)'!$A$8</f>
@@ -3577,7 +3577,7 @@
         <v>9</v>
       </c>
       <c r="I10" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="J10" t="s">
         <v>7</v>
@@ -3601,7 +3601,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E11" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F11" t="str">
         <f>'BusbarSection(5)'!$A$11</f>
@@ -3615,7 +3615,7 @@
         <v>10</v>
       </c>
       <c r="I11" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="J11" t="s">
         <v>19</v>
@@ -3639,7 +3639,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E12" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F12" t="str">
         <f>'BusbarSection(5)'!$A$11</f>
@@ -3653,7 +3653,7 @@
         <v>11</v>
       </c>
       <c r="I12" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="J12" t="s">
         <v>19</v>
@@ -3677,7 +3677,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E13" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F13" t="str">
         <f>'Bay(4)'!$A$7</f>
@@ -3691,7 +3691,7 @@
         <v>12</v>
       </c>
       <c r="I13" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="J13" t="s">
         <v>6</v>
@@ -3715,7 +3715,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E14" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F14" t="str">
         <f>'Bay(4)'!$A$7</f>
@@ -3729,7 +3729,7 @@
         <v>13</v>
       </c>
       <c r="I14" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="J14" t="s">
         <v>6</v>
@@ -3753,7 +3753,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E15" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F15" t="str">
         <f>'Bay(4)'!$A$7</f>
@@ -3767,7 +3767,7 @@
         <v>14</v>
       </c>
       <c r="I15" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="J15" t="s">
         <v>6</v>
@@ -3791,7 +3791,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E16" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F16" t="str">
         <f>'Bay(4)'!$A$7</f>
@@ -3805,7 +3805,7 @@
         <v>15</v>
       </c>
       <c r="I16" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="J16" t="s">
         <v>6</v>
@@ -3829,7 +3829,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E17" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F17" t="str">
         <f>'Bay(4)'!$A$7</f>
@@ -3843,7 +3843,7 @@
         <v>16</v>
       </c>
       <c r="I17" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="J17" t="s">
         <v>6</v>
@@ -3867,7 +3867,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E18" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F18" t="str">
         <f>'Bay(4)'!$A$7</f>
@@ -3881,7 +3881,7 @@
         <v>17</v>
       </c>
       <c r="I18" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="J18" t="s">
         <v>6</v>
@@ -3905,7 +3905,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E19" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F19" t="str">
         <f>'Bay(4)'!$A$7</f>
@@ -3919,7 +3919,7 @@
         <v>18</v>
       </c>
       <c r="I19" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="J19" t="s">
         <v>6</v>
@@ -3943,7 +3943,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E20" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F20" t="str">
         <f>'Bay(4)'!$A$2</f>
@@ -3957,7 +3957,7 @@
         <v>19</v>
       </c>
       <c r="I20" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="J20" t="s">
         <v>8</v>
@@ -3981,7 +3981,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E21" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F21" t="str">
         <f>'Bay(4)'!$A$3</f>
@@ -3995,7 +3995,7 @@
         <v>20</v>
       </c>
       <c r="I21" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="J21" t="s">
         <v>9</v>
@@ -4019,7 +4019,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E22" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F22" t="str">
         <f>'Bay(4)'!$A$2</f>
@@ -4033,7 +4033,7 @@
         <v>21</v>
       </c>
       <c r="I22" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="J22" t="s">
         <v>8</v>
@@ -4057,7 +4057,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E23" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F23" t="str">
         <f>'Bay(4)'!$A$3</f>
@@ -4071,7 +4071,7 @@
         <v>22</v>
       </c>
       <c r="I23" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="J23" t="s">
         <v>9</v>
@@ -4095,7 +4095,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E24" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F24" t="str">
         <f>'Bay(4)'!$A$4</f>
@@ -4109,7 +4109,7 @@
         <v>23</v>
       </c>
       <c r="I24" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="J24" t="s">
         <v>3</v>
@@ -4133,7 +4133,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E25" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F25" t="str">
         <f>'Bay(4)'!$A$4</f>
@@ -4147,7 +4147,7 @@
         <v>24</v>
       </c>
       <c r="I25" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="J25" t="s">
         <v>3</v>
@@ -4171,7 +4171,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E26" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F26" t="str">
         <f>'Bay(4)'!$A$4</f>
@@ -4185,7 +4185,7 @@
         <v>25</v>
       </c>
       <c r="I26" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="J26" t="s">
         <v>3</v>
@@ -4209,7 +4209,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E27" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F27" t="str">
         <f>'Bay(4)'!$A$4</f>
@@ -4223,7 +4223,7 @@
         <v>26</v>
       </c>
       <c r="I27" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="J27" t="s">
         <v>3</v>
@@ -4247,7 +4247,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E28" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F28" t="str">
         <f>'Bay(4)'!$A$4</f>
@@ -4261,7 +4261,7 @@
         <v>27</v>
       </c>
       <c r="I28" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="J28" t="s">
         <v>3</v>
@@ -4285,7 +4285,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E29" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F29" t="str">
         <f>'Bay(4)'!$A$5</f>
@@ -4299,7 +4299,7 @@
         <v>28</v>
       </c>
       <c r="I29" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="J29" t="s">
         <v>4</v>
@@ -4323,7 +4323,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E30" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F30" t="str">
         <f>'Bay(4)'!$A$5</f>
@@ -4337,7 +4337,7 @@
         <v>29</v>
       </c>
       <c r="I30" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="J30" t="s">
         <v>4</v>
@@ -4361,7 +4361,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E31" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F31" t="str">
         <f>'Bay(4)'!$A$5</f>
@@ -4375,7 +4375,7 @@
         <v>30</v>
       </c>
       <c r="I31" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="J31" t="s">
         <v>4</v>
@@ -4399,7 +4399,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E32" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F32" t="str">
         <f>'Bay(4)'!$A$5</f>
@@ -4413,7 +4413,7 @@
         <v>31</v>
       </c>
       <c r="I32" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="J32" t="s">
         <v>4</v>
@@ -4437,7 +4437,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E33" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F33" t="str">
         <f>'Bay(4)'!$A$5</f>
@@ -4451,7 +4451,7 @@
         <v>32</v>
       </c>
       <c r="I33" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="J33" t="s">
         <v>4</v>
@@ -4475,7 +4475,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E34" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F34" t="str">
         <f>'Bay(4)'!$A$5</f>
@@ -4489,7 +4489,7 @@
         <v>33</v>
       </c>
       <c r="I34" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="J34" t="s">
         <v>4</v>
@@ -4513,7 +4513,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E35" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F35" t="str">
         <f>'Bay(4)'!$A$5</f>
@@ -4527,7 +4527,7 @@
         <v>34</v>
       </c>
       <c r="I35" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="J35" t="s">
         <v>4</v>
@@ -4551,7 +4551,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E36" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F36" t="str">
         <f>'Bay(4)'!$A$5</f>
@@ -4565,7 +4565,7 @@
         <v>35</v>
       </c>
       <c r="I36" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="J36" t="s">
         <v>4</v>
@@ -4589,7 +4589,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E37" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F37" t="str">
         <f>'Bay(4)'!$A$5</f>
@@ -4603,7 +4603,7 @@
         <v>36</v>
       </c>
       <c r="I37" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="J37" t="s">
         <v>4</v>
@@ -4627,7 +4627,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E38" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F38" t="str">
         <f>'Bay(4)'!$A$6</f>
@@ -4641,7 +4641,7 @@
         <v>37</v>
       </c>
       <c r="I38" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="J38" t="s">
         <v>5</v>
@@ -4665,7 +4665,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E39" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F39" t="str">
         <f>'Bay(4)'!$A$6</f>
@@ -4679,7 +4679,7 @@
         <v>38</v>
       </c>
       <c r="I39" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="J39" t="s">
         <v>5</v>
@@ -4703,7 +4703,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E40" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F40" t="str">
         <f>'Bay(4)'!$A$6</f>
@@ -4717,7 +4717,7 @@
         <v>39</v>
       </c>
       <c r="I40" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="J40" t="s">
         <v>5</v>
@@ -4741,7 +4741,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E41" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F41" t="str">
         <f>'Bay(4)'!$A$6</f>
@@ -4755,7 +4755,7 @@
         <v>40</v>
       </c>
       <c r="I41" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="J41" t="s">
         <v>5</v>
@@ -4779,7 +4779,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E42" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F42" t="str">
         <f>'Bay(4)'!$A$6</f>
@@ -4793,7 +4793,7 @@
         <v>41</v>
       </c>
       <c r="I42" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="J42" t="s">
         <v>5</v>
@@ -4817,7 +4817,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E43" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F43" t="str">
         <f>'Bay(4)'!$A$6</f>
@@ -4831,7 +4831,7 @@
         <v>42</v>
       </c>
       <c r="I43" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="J43" t="s">
         <v>5</v>
@@ -4855,7 +4855,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E44" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F44" t="str">
         <f>'Bay(4)'!$A$6</f>
@@ -4869,7 +4869,7 @@
         <v>43</v>
       </c>
       <c r="I44" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="J44" t="s">
         <v>5</v>
@@ -4893,7 +4893,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E45" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F45" t="str">
         <f>'Bay(4)'!$A$6</f>
@@ -4907,7 +4907,7 @@
         <v>44</v>
       </c>
       <c r="I45" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="J45" t="s">
         <v>5</v>
@@ -4931,7 +4931,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E46" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F46" t="str">
         <f>'Bay(4)'!$A$6</f>
@@ -4945,7 +4945,7 @@
         <v>45</v>
       </c>
       <c r="I46" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="J46" t="s">
         <v>5</v>
@@ -4969,7 +4969,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E47" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F47" t="str">
         <f>'BusbarSection(5)'!$A$2</f>
@@ -4983,7 +4983,7 @@
         <v>46</v>
       </c>
       <c r="I47" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="J47" t="s">
         <v>16</v>
@@ -5007,7 +5007,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E48" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F48" t="str">
         <f>'BusbarSection(5)'!$A$3</f>
@@ -5021,7 +5021,7 @@
         <v>47</v>
       </c>
       <c r="I48" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="J48" t="s">
         <v>18</v>
@@ -5045,7 +5045,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E49" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F49" t="str">
         <f>'Bay(4)'!$A$2</f>
@@ -5059,7 +5059,7 @@
         <v>48</v>
       </c>
       <c r="I49" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="J49" t="s">
         <v>8</v>
@@ -5083,7 +5083,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E50" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F50" t="str">
         <f>'Bay(4)'!$A$3</f>
@@ -5097,7 +5097,7 @@
         <v>49</v>
       </c>
       <c r="I50" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="J50" t="s">
         <v>9</v>
@@ -5121,7 +5121,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E51" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F51" t="str">
         <f>'Bay(4)'!$A$13</f>
@@ -5135,7 +5135,7 @@
         <v>50</v>
       </c>
       <c r="I51" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="J51" t="s">
         <v>14</v>
@@ -5159,7 +5159,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E52" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F52" t="str">
         <f>'Bay(4)'!$A$11</f>
@@ -5173,7 +5173,7 @@
         <v>51</v>
       </c>
       <c r="I52" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="J52" t="s">
         <v>12</v>
@@ -5197,7 +5197,7 @@
         <v>_96521323C5CB419BA6433904BBAFC08B</v>
       </c>
       <c r="E53" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="F53" t="str">
         <f>'Bay(4)'!$A$12</f>
@@ -5211,7 +5211,7 @@
         <v>52</v>
       </c>
       <c r="I53" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="J53" t="s">
         <v>13</v>
@@ -5242,28 +5242,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -5291,7 +5291,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="H2" t="s">
         <v>6</v>
@@ -5322,7 +5322,7 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="H3" t="s">
         <v>7</v>
@@ -5353,7 +5353,7 @@
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="H4" t="s">
         <v>6</v>
@@ -5384,7 +5384,7 @@
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="H5" t="s">
         <v>6</v>
@@ -5415,7 +5415,7 @@
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="H6" t="s">
         <v>7</v>
@@ -5446,7 +5446,7 @@
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="H7" t="s">
         <v>7</v>
@@ -5477,7 +5477,7 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="H8" t="s">
         <v>4</v>
@@ -5508,7 +5508,7 @@
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="H9" t="s">
         <v>5</v>
@@ -5539,10 +5539,10 @@
         <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="H10" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -5570,10 +5570,10 @@
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="H11" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -5601,10 +5601,10 @@
         <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="H12" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -5632,10 +5632,10 @@
         <v>12</v>
       </c>
       <c r="G13" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="H13" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -5663,7 +5663,7 @@
         <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="H14" t="s">
         <v>12</v>
@@ -5694,7 +5694,7 @@
         <v>14</v>
       </c>
       <c r="G15" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="H15" t="s">
         <v>12</v>
@@ -5725,7 +5725,7 @@
         <v>15</v>
       </c>
       <c r="G16" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="H16" t="s">
         <v>13</v>
@@ -5756,7 +5756,7 @@
         <v>16</v>
       </c>
       <c r="G17" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="H17" t="s">
         <v>13</v>
@@ -5787,7 +5787,7 @@
         <v>17</v>
       </c>
       <c r="G18" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="H18" t="s">
         <v>14</v>
@@ -5818,7 +5818,7 @@
         <v>18</v>
       </c>
       <c r="G19" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="H19" t="s">
         <v>14</v>
@@ -5849,28 +5849,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -5898,10 +5898,10 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="H2" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -5929,10 +5929,10 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="H3" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -5960,10 +5960,10 @@
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="H4" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -5991,10 +5991,10 @@
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="H5" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -6078,10 +6078,10 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="H8" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -6109,10 +6109,10 @@
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="H9" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -6234,56 +6234,92 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
     <col min="3" max="3" width="48.42578125" customWidth="1"/>
-    <col min="4" max="4" width="48.140625" customWidth="1"/>
-    <col min="5" max="5" width="43.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" customWidth="1"/>
-    <col min="7" max="7" width="49.28515625" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" customWidth="1"/>
+    <col min="5" max="6" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22" customWidth="1"/>
+    <col min="11" max="11" width="26.28515625" customWidth="1"/>
+    <col min="12" max="12" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="34" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="40.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>84</v>
+      <c r="P1" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>format_template!$B$2&amp;E2&amp;format_template!$C$2&amp;F2</f>
         <v>_1_3</v>
       </c>
       <c r="B2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C2" t="s">
         <v>44</v>
       </c>
-      <c r="C2" t="s">
-        <v>45</v>
-      </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2">
         <f>format_template!$B$5</f>
@@ -6293,19 +6329,19 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>format_template!$B$2&amp;E3&amp;format_template!$C$2&amp;F3</f>
         <v>_1_7</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>216</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E3">
         <f>format_template!$B$5</f>
@@ -6314,20 +6350,24 @@
       <c r="F3">
         <v>7</v>
       </c>
+      <c r="G3" t="str">
+        <f>A2</f>
+        <v>_1_3</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>format_template!$B$2&amp;E4&amp;format_template!$C$2&amp;F4</f>
         <v>_1_11</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>217</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E4">
         <f>format_template!$B$5</f>
@@ -6337,19 +6377,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>format_template!$B$2&amp;E5&amp;format_template!$C$2&amp;F5</f>
         <v>_1_15</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>217</v>
       </c>
       <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
         <v>52</v>
-      </c>
-      <c r="D5" t="s">
-        <v>59</v>
       </c>
       <c r="E5">
         <f>format_template!$B$5</f>
@@ -6358,20 +6398,32 @@
       <c r="F5">
         <v>15</v>
       </c>
+      <c r="H5" t="str">
+        <f>A6</f>
+        <v>_1_19</v>
+      </c>
+      <c r="I5" t="str">
+        <f>A4</f>
+        <v>_1_11</v>
+      </c>
+      <c r="K5" t="str">
+        <f>A3</f>
+        <v>_1_7</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>format_template!$B$2&amp;E6&amp;format_template!$C$2&amp;F6</f>
         <v>_1_19</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>218</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="E6">
         <f>format_template!$B$5</f>
@@ -6381,19 +6433,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>format_template!$B$2&amp;E7&amp;format_template!$C$2&amp;F7</f>
         <v>_1_23</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>217</v>
       </c>
       <c r="C7" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D7" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="E7">
         <f>format_template!$B$5</f>
@@ -6402,20 +6454,28 @@
       <c r="F7">
         <v>23</v>
       </c>
+      <c r="H7" t="str">
+        <f>A8</f>
+        <v>_1_27</v>
+      </c>
+      <c r="I7" t="str">
+        <f>A5</f>
+        <v>_1_15</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>format_template!$B$2&amp;E8&amp;format_template!$C$2&amp;F8</f>
         <v>_1_27</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>218</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E8">
         <f>format_template!$B$5</f>
@@ -6425,19 +6485,19 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>format_template!$B$2&amp;E9&amp;format_template!$C$2&amp;F9</f>
         <v>_1_31</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>219</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E9">
         <f>format_template!$B$5</f>
@@ -6446,20 +6506,24 @@
       <c r="F9">
         <v>31</v>
       </c>
+      <c r="J9" t="str">
+        <f>A11</f>
+        <v>_1_39</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>format_template!$B$2&amp;E10&amp;format_template!$C$2&amp;F10</f>
         <v>_1_35</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>219</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E10">
         <f>format_template!$B$5</f>
@@ -6468,20 +6532,24 @@
       <c r="F10">
         <v>35</v>
       </c>
+      <c r="J10" t="str">
+        <f>A2</f>
+        <v>_1_3</v>
+      </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>format_template!$B$2&amp;E11&amp;format_template!$C$2&amp;F11</f>
         <v>_1_39</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>220</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E11">
         <f>format_template!$B$5</f>
@@ -6491,19 +6559,19 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>format_template!$B$2&amp;E12&amp;format_template!$C$2&amp;F12</f>
         <v>_1_43</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>221</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E12">
         <f>format_template!$B$5</f>
@@ -6512,169 +6580,22 @@
       <c r="F12">
         <v>43</v>
       </c>
-      <c r="G12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C17" t="str">
-        <f>D5</f>
-        <v>филиал ПАО «ФСК ЕЭС» – МЭС Северо-Запада</v>
-      </c>
-      <c r="D17" t="str">
-        <f>A5</f>
-        <v>_1_15</v>
-      </c>
-      <c r="E17" t="s">
-        <v>73</v>
-      </c>
-      <c r="F17" t="str">
-        <f>A6</f>
-        <v>_1_19</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E18" t="s">
-        <v>74</v>
-      </c>
-      <c r="F18" t="str">
-        <f>A4</f>
-        <v>_1_11</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E19" t="s">
-        <v>75</v>
-      </c>
-      <c r="F19" t="str">
+      <c r="L12" t="str">
         <f>A3</f>
         <v>_1_7</v>
       </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" t="str">
-        <f>D7</f>
-        <v>Новгородское ПМЭС</v>
-      </c>
-      <c r="D21" t="str">
+      <c r="M12" t="s">
+        <v>36</v>
+      </c>
+      <c r="N12" t="str">
         <f>A7</f>
         <v>_1_23</v>
       </c>
-      <c r="E21" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" t="str">
-        <f>A8</f>
-        <v>_1_27</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E22" t="s">
-        <v>74</v>
-      </c>
-      <c r="F22" t="str">
-        <f>A5</f>
-        <v>_1_15</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" t="str">
-        <f>D9</f>
-        <v>ЦУС Северо-Запада</v>
-      </c>
-      <c r="D25" t="str">
-        <f>A5</f>
-        <v>_1_15</v>
-      </c>
-      <c r="E25" t="s">
-        <v>76</v>
-      </c>
-      <c r="F25" t="str">
-        <f>A11</f>
-        <v>_1_39</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" t="str">
-        <f>D10</f>
-        <v>РДУ Северо-Запада</v>
-      </c>
-      <c r="D27" t="str">
-        <f>A10</f>
-        <v>_1_35</v>
-      </c>
-      <c r="E27" t="s">
-        <v>76</v>
-      </c>
-      <c r="F27" t="str">
-        <f>A2</f>
-        <v>_1_3</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" t="str">
-        <f>D12</f>
-        <v>ПС 500 Белобережская</v>
-      </c>
-      <c r="D30" t="str">
-        <f>A12</f>
-        <v>_1_43</v>
-      </c>
-      <c r="E30" t="s">
-        <v>69</v>
-      </c>
-      <c r="F30" t="str">
-        <f>A3</f>
-        <v>_1_7</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E31" t="s">
-        <v>70</v>
-      </c>
-      <c r="F31" t="str">
-        <f>G12</f>
-        <v>_4389F40360A14925B33ACB46E59F47F0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E32" t="s">
-        <v>71</v>
-      </c>
-      <c r="F32" t="str">
-        <f>A7</f>
-        <v>_1_23</v>
-      </c>
-    </row>
-    <row r="33" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E33" t="s">
-        <v>72</v>
-      </c>
-      <c r="F33" t="str">
+      <c r="O12" t="str">
         <f>A9</f>
         <v>_1_31</v>
       </c>
-    </row>
-    <row r="34" spans="5:6" x14ac:dyDescent="0.25">
-      <c r="E34" t="s">
-        <v>72</v>
-      </c>
-      <c r="F34" t="str">
+      <c r="P12" t="str">
         <f>A10</f>
         <v>_1_35</v>
       </c>
@@ -6690,7 +6611,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6699,33 +6620,33 @@
     <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="54.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="34.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>82</v>
+        <v>214</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -6734,10 +6655,10 @@
         <v>_2_1</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D2">
         <v>15</v>
@@ -6762,10 +6683,10 @@
         <v>_2_2</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="D3">
         <v>8</v>
@@ -6790,10 +6711,10 @@
         <v>_2_3</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="E4" s="4">
         <v>10</v>
@@ -6815,13 +6736,13 @@
         <v>_2_4</v>
       </c>
       <c r="B5" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="C5" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="F5">
         <v>13948116</v>
@@ -6845,7 +6766,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6861,26 +6782,26 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -6970,10 +6891,10 @@
         <v>_3_4</v>
       </c>
       <c r="B5" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C5" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="D5" t="str">
         <f>'BaseVoltage(2)'!$A$5</f>
@@ -7015,22 +6936,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -7355,22 +7276,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -7616,7 +7537,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7629,16 +7550,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -7654,7 +7575,7 @@
         <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -7668,7 +7589,7 @@
         <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -7682,7 +7603,7 @@
         <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -7696,7 +7617,7 @@
         <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -7722,8 +7643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7738,28 +7659,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -7771,7 +7692,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="D2">
         <v>250</v>
@@ -7801,7 +7722,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="D3">
         <v>250</v>
@@ -7831,7 +7752,7 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="E4" t="str">
         <f>PSRType!$A$3</f>
@@ -7858,7 +7779,7 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="E5" t="str">
         <f>PSRType!$A$3</f>
@@ -7909,55 +7830,55 @@
   <sheetData>
     <row r="1" spans="1:16383" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
@@ -24355,10 +24276,10 @@
         <v>1</v>
       </c>
       <c r="P2" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="Q2" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:16383" x14ac:dyDescent="0.25">
@@ -24390,10 +24311,10 @@
         <v>2</v>
       </c>
       <c r="P3" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="Q3" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:16383" x14ac:dyDescent="0.25">
@@ -24425,10 +24346,10 @@
         <v>3</v>
       </c>
       <c r="P4" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="Q4" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:16383" x14ac:dyDescent="0.25">
@@ -24460,10 +24381,10 @@
         <v>4</v>
       </c>
       <c r="P5" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="Q5" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:16383" x14ac:dyDescent="0.25">
@@ -24495,10 +24416,10 @@
         <v>5</v>
       </c>
       <c r="P6" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="Q6" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:16383" x14ac:dyDescent="0.25">
@@ -24530,10 +24451,10 @@
         <v>6</v>
       </c>
       <c r="P7" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="Q7" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
     </row>
     <row r="8" spans="1:16383" x14ac:dyDescent="0.25">
@@ -24568,7 +24489,7 @@
         <v>12</v>
       </c>
       <c r="Q8" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:16383" x14ac:dyDescent="0.25">
@@ -24603,7 +24524,7 @@
         <v>12</v>
       </c>
       <c r="Q9" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
     </row>
     <row r="10" spans="1:16383" x14ac:dyDescent="0.25">
@@ -24638,7 +24559,7 @@
         <v>13</v>
       </c>
       <c r="Q10" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:16383" x14ac:dyDescent="0.25">
@@ -24673,7 +24594,7 @@
         <v>13</v>
       </c>
       <c r="Q11" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>